<commit_message>
fix login bug and now merchant admin merchant add finished
</commit_message>
<xml_diff>
--- a/document/数据库设计（fan）.xlsx
+++ b/document/数据库设计（fan）.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139">
   <si>
     <t>字段</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>教育部认证</t>
+  </si>
+  <si>
+    <t>willing_to_cooperate</t>
+  </si>
+  <si>
+    <t>是否愿意合作</t>
   </si>
   <si>
     <t>String</t>
@@ -441,11 +447,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,15 +471,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -484,39 +482,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -537,8 +504,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,15 +527,29 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -583,8 +572,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,9 +590,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -605,6 +603,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -615,13 +628,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,61 +778,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,103 +802,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,26 +819,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -847,8 +840,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,21 +894,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -906,6 +908,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -914,10 +927,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -926,137 +939,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1067,6 +1080,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1387,10 +1403,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1993,17 +2009,31 @@
       <c r="A48" t="s">
         <v>103</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C48" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2085,15 +2115,15 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2101,7 +2131,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2109,7 +2139,7 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2117,23 +2147,23 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2141,7 +2171,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2171,7 +2201,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2191,10 +2221,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -2206,7 +2236,7 @@
     <row r="3" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -2215,7 +2245,7 @@
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>30</v>
@@ -2224,7 +2254,7 @@
     <row r="5" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
@@ -2233,7 +2263,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>30</v>
@@ -2242,7 +2272,7 @@
     <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>30</v>
@@ -2251,7 +2281,7 @@
     <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>30</v>
@@ -2260,7 +2290,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>30</v>
@@ -2269,7 +2299,7 @@
     <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>30</v>
@@ -2278,7 +2308,7 @@
     <row r="11" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>30</v>
@@ -2287,7 +2317,7 @@
     <row r="12" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
@@ -2296,7 +2326,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -2305,7 +2335,7 @@
     <row r="14" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>30</v>
@@ -2314,7 +2344,7 @@
     <row r="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>30</v>
@@ -2323,7 +2353,7 @@
     <row r="16" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>63</v>
@@ -2332,7 +2362,7 @@
     <row r="17" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -2341,7 +2371,7 @@
     <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>63</v>
@@ -2355,7 +2385,7 @@
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>63</v>
@@ -2369,7 +2399,7 @@
     <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>63</v>
@@ -2378,7 +2408,7 @@
     <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
@@ -2387,7 +2417,7 @@
     <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>26</v>
@@ -2396,7 +2426,7 @@
     <row r="25" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>26</v>
@@ -2405,7 +2435,7 @@
     <row r="26" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
@@ -2414,7 +2444,7 @@
     <row r="27" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add ban in merchant model
</commit_message>
<xml_diff>
--- a/document/数据库设计（fan）.xlsx
+++ b/document/数据库设计（fan）.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142">
   <si>
     <t>字段</t>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>是否愿意合作</t>
+  </si>
+  <si>
+    <t>banned</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>封号处理</t>
   </si>
   <si>
     <t>String</t>
@@ -446,12 +455,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,34 +478,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -513,14 +500,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -528,21 +515,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,6 +541,13 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -567,6 +562,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -590,22 +600,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -613,7 +608,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,25 +630,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,157 +756,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -822,17 +824,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,24 +844,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,6 +864,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -909,13 +907,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -927,10 +929,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -939,19 +941,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -960,116 +962,116 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1080,9 +1082,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1403,10 +1402,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -2009,13 +2008,13 @@
       <c r="A48" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C48" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -2026,7 +2025,7 @@
       <c r="A49" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C49" t="s">
@@ -2034,6 +2033,20 @@
       </c>
       <c r="D49" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2115,15 +2128,15 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2131,7 +2144,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2139,7 +2152,7 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2147,23 +2160,23 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
         <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2171,7 +2184,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2201,7 +2214,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2221,10 +2234,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -2236,7 +2249,7 @@
     <row r="3" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -2245,7 +2258,7 @@
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>30</v>
@@ -2254,7 +2267,7 @@
     <row r="5" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
@@ -2263,7 +2276,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>30</v>
@@ -2272,7 +2285,7 @@
     <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>30</v>
@@ -2281,7 +2294,7 @@
     <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>30</v>
@@ -2290,7 +2303,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>30</v>
@@ -2299,7 +2312,7 @@
     <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>30</v>
@@ -2308,7 +2321,7 @@
     <row r="11" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>30</v>
@@ -2317,7 +2330,7 @@
     <row r="12" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
@@ -2326,7 +2339,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -2335,7 +2348,7 @@
     <row r="14" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>30</v>
@@ -2344,7 +2357,7 @@
     <row r="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>30</v>
@@ -2353,7 +2366,7 @@
     <row r="16" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>63</v>
@@ -2362,7 +2375,7 @@
     <row r="17" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -2371,7 +2384,7 @@
     <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>63</v>
@@ -2385,7 +2398,7 @@
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>63</v>
@@ -2399,7 +2412,7 @@
     <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>63</v>
@@ -2408,7 +2421,7 @@
     <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
@@ -2417,7 +2430,7 @@
     <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>26</v>
@@ -2426,7 +2439,7 @@
     <row r="25" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>26</v>
@@ -2435,7 +2448,7 @@
     <row r="26" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
@@ -2444,7 +2457,7 @@
     <row r="27" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
new merchant create task finish
</commit_message>
<xml_diff>
--- a/document/数据库设计（fan）.xlsx
+++ b/document/数据库设计（fan）.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14085"/>
+    <workbookView windowWidth="28695" windowHeight="14070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="商户信息表" sheetId="1" r:id="rId1"/>
-    <sheet name="收藏信息表" sheetId="2" r:id="rId2"/>
-    <sheet name="评论信息表" sheetId="3" r:id="rId3"/>
-    <sheet name="管理员信息表" sheetId="4" r:id="rId4"/>
-    <sheet name="用户信息表" sheetId="5" r:id="rId5"/>
-    <sheet name="教师信息表" sheetId="6" r:id="rId6"/>
-    <sheet name="可选套餐表" sheetId="7" r:id="rId7"/>
-    <sheet name="订单表" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
+    <sheet name="管理员任务表" sheetId="2" r:id="rId2"/>
+    <sheet name="收藏信息表" sheetId="3" r:id="rId3"/>
+    <sheet name="评论信息表" sheetId="4" r:id="rId4"/>
+    <sheet name="管理员信息表" sheetId="5" r:id="rId5"/>
+    <sheet name="用户信息表" sheetId="6" r:id="rId6"/>
+    <sheet name="教师信息表" sheetId="7" r:id="rId7"/>
+    <sheet name="可选套餐表" sheetId="8" r:id="rId8"/>
+    <sheet name="订单表" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167">
   <si>
     <t>字段</t>
   </si>
@@ -99,87 +99,81 @@
     <t>购买的用户</t>
   </si>
   <si>
-    <t>reputation</t>
+    <t>hierarchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> String</t>
+  </si>
+  <si>
+    <t>商户重要级别</t>
+  </si>
+  <si>
+    <t>管理员创建</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>商户名称</t>
+  </si>
+  <si>
+    <t>管理员创建或者商户注册</t>
+  </si>
+  <si>
+    <t>contact_person_name</t>
+  </si>
+  <si>
+    <t>商户联系人</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>商户联系邮箱</t>
+  </si>
+  <si>
+    <t>商户注册需进行邮箱验证</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>商户登录密码</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>商户联系电话</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>商户网站</t>
+  </si>
+  <si>
+    <t>商户上线前商户中心添加</t>
+  </si>
+  <si>
+    <t>follow_up_people</t>
+  </si>
+  <si>
+    <t>跟进的管理员</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> String（admin_id）</t>
+  </si>
+  <si>
+    <t>管理员ID</t>
+  </si>
+  <si>
+    <t>live</t>
   </si>
   <si>
     <t xml:space="preserve"> Boolean</t>
   </si>
   <si>
-    <t xml:space="preserve">是否可合作 </t>
-  </si>
-  <si>
-    <t>管理员创建</t>
-  </si>
-  <si>
-    <t>hierarchy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> String</t>
-  </si>
-  <si>
-    <t>商户重要级别</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>商户名称</t>
-  </si>
-  <si>
-    <t>管理员创建或者商户注册</t>
-  </si>
-  <si>
-    <t>contact_person_name</t>
-  </si>
-  <si>
-    <t>商户联系人</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>商户联系邮箱</t>
-  </si>
-  <si>
-    <t>商户注册需进行邮箱验证</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>商户登录密码</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>商户联系电话</t>
-  </si>
-  <si>
-    <t>website</t>
-  </si>
-  <si>
-    <t>商户网站</t>
-  </si>
-  <si>
-    <t>商户上线前商户中心添加</t>
-  </si>
-  <si>
-    <t>follow_up_people</t>
-  </si>
-  <si>
-    <t>跟进的管理员</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> String（admin_id）</t>
-  </si>
-  <si>
-    <t>管理员ID</t>
-  </si>
-  <si>
-    <t>live</t>
-  </si>
-  <si>
     <t>是否可以上线显示给用户</t>
   </si>
   <si>
@@ -354,9 +348,96 @@
     <t>封号处理</t>
   </si>
   <si>
+    <t>可选值</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
     <t>String</t>
   </si>
   <si>
+    <t>标题</t>
+  </si>
+  <si>
+    <t>生成时默认显示或管理员创建</t>
+  </si>
+  <si>
+    <t>merchant</t>
+  </si>
+  <si>
+    <t>商户信息</t>
+  </si>
+  <si>
+    <t>创建商户时候生成</t>
+  </si>
+  <si>
+    <t>id: Number</t>
+  </si>
+  <si>
+    <t>商户id</t>
+  </si>
+  <si>
+    <t>hierarchy: String</t>
+  </si>
+  <si>
+    <t>商户等级</t>
+  </si>
+  <si>
+    <t>willing_to_cooperate: Boolean</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>管理员名字</t>
+  </si>
+  <si>
+    <t>创建任务时候生成</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>"SignUpMerchant"</t>
+  </si>
+  <si>
+    <t>"InternalTask"</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>任务状态</t>
+  </si>
+  <si>
+    <t>"initial"</t>
+  </si>
+  <si>
+    <t>"Handling"</t>
+  </si>
+  <si>
+    <t>"Finish"</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>创建时间</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>content: String,</t>
+  </si>
+  <si>
+    <t>内容</t>
+  </si>
+  <si>
+    <t>create_time: Date</t>
+  </si>
+  <si>
     <t>response_company</t>
   </si>
   <si>
@@ -364,12 +445,6 @@
   </si>
   <si>
     <t>birthday</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>表名</t>
@@ -455,12 +530,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,6 +553,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -485,7 +567,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -506,18 +596,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -528,47 +611,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,9 +642,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,7 +690,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -636,181 +718,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,11 +906,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -853,17 +941,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,6 +961,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -906,21 +1003,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -929,10 +1011,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -941,137 +1023,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1082,6 +1164,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1402,10 +1487,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1551,7 +1636,7 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1560,13 +1645,13 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1574,194 +1659,191 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
       <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="D20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" t="s">
         <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -1772,18 +1854,21 @@
         <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="B31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1791,49 +1876,52 @@
         <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1841,16 +1929,16 @@
         <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1858,100 +1946,94 @@
         <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>46</v>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" t="s">
         <v>84</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
+      <c r="D40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="41" spans="2:4">
       <c r="B41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" t="s">
         <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="2:4">
       <c r="B42" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
         <v>91</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" t="s">
         <v>92</v>
-      </c>
-      <c r="B43" t="s">
-        <v>63</v>
       </c>
       <c r="C43" t="s">
         <v>93</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -1962,7 +2044,7 @@
         <v>95</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -1973,80 +2055,69 @@
         <v>97</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>46</v>
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>100</v>
-      </c>
-      <c r="B47" t="s">
-        <v>26</v>
+        <v>101</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="D47" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>103</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>90</v>
+      <c r="D48" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>26</v>
+      <c r="B49" t="s">
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
         <v>107</v>
       </c>
-      <c r="B50" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" t="s">
-        <v>53</v>
+      <c r="D49" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2057,6 +2128,191 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="31.125" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="36.875" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="24.125" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1"/>
@@ -2072,7 +2328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1"/>
@@ -2088,7 +2344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:F9"/>
@@ -2125,7 +2381,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>110</v>
@@ -2133,15 +2389,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>110</v>
@@ -2149,7 +2405,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>110</v>
@@ -2157,7 +2413,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
@@ -2165,7 +2421,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>110</v>
@@ -2173,7 +2429,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
         <v>110</v>
@@ -2184,7 +2440,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2193,7 +2449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:F27"/>
@@ -2214,7 +2470,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2234,10 +2490,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -2249,7 +2505,7 @@
     <row r="3" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -2258,88 +2514,88 @@
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -2348,34 +2604,34 @@
     <row r="14" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -2384,10 +2640,10 @@
     <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2398,10 +2654,10 @@
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2412,16 +2668,16 @@
     <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
@@ -2430,25 +2686,25 @@
     <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
@@ -2457,29 +2713,13 @@
     <row r="27" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
@@ -2496,7 +2736,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2528,7 +2768,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish get admin response merchant
</commit_message>
<xml_diff>
--- a/document/数据库设计（fan）.xlsx
+++ b/document/数据库设计（fan）.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168">
   <si>
     <t>字段</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>willing_to_cooperate: Boolean</t>
+  </si>
+  <si>
+    <t>商户名</t>
   </si>
   <si>
     <t>admin</t>
@@ -532,10 +535,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,13 +548,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -575,7 +571,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -596,23 +592,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -626,26 +607,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -659,9 +625,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -688,16 +654,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -712,6 +708,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -719,180 +889,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,6 +899,69 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -917,15 +976,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,60 +999,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1011,10 +1007,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1023,137 +1019,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1164,9 +1160,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2085,7 +2078,7 @@
       <c r="C47" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -2130,10 +2123,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2214,96 +2207,104 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>122</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>124</v>
       </c>
       <c r="B8" t="s">
         <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>125</v>
-      </c>
-      <c r="F8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>127</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
       </c>
       <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
         <v>129</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
         <v>130</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="G10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>135</v>
-      </c>
-      <c r="C12" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
         <v>137</v>
       </c>
-      <c r="C13" t="s">
-        <v>133</v>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2389,10 +2390,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2421,7 +2422,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
         <v>110</v>
@@ -2429,7 +2430,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
         <v>110</v>
@@ -2440,7 +2441,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2470,7 +2471,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2490,10 +2491,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -2505,7 +2506,7 @@
     <row r="3" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -2514,7 +2515,7 @@
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>26</v>
@@ -2523,7 +2524,7 @@
     <row r="5" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>26</v>
@@ -2532,7 +2533,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>26</v>
@@ -2541,7 +2542,7 @@
     <row r="7" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>26</v>
@@ -2550,7 +2551,7 @@
     <row r="8" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>26</v>
@@ -2559,7 +2560,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>26</v>
@@ -2568,7 +2569,7 @@
     <row r="10" spans="1:3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>26</v>
@@ -2577,7 +2578,7 @@
     <row r="11" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>26</v>
@@ -2586,7 +2587,7 @@
     <row r="12" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>26</v>
@@ -2595,7 +2596,7 @@
     <row r="13" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
@@ -2604,7 +2605,7 @@
     <row r="14" spans="1:3">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>26</v>
@@ -2613,7 +2614,7 @@
     <row r="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>26</v>
@@ -2622,7 +2623,7 @@
     <row r="16" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>61</v>
@@ -2631,7 +2632,7 @@
     <row r="17" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -2640,7 +2641,7 @@
     <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>61</v>
@@ -2654,7 +2655,7 @@
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>61</v>
@@ -2668,7 +2669,7 @@
     <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>61</v>
@@ -2677,7 +2678,7 @@
     <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>14</v>
@@ -2686,7 +2687,7 @@
     <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>49</v>
@@ -2695,7 +2696,7 @@
     <row r="25" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>49</v>
@@ -2704,7 +2705,7 @@
     <row r="26" spans="1:3">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
@@ -2713,7 +2714,7 @@
     <row r="27" spans="1:3">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
user login register finished
</commit_message>
<xml_diff>
--- a/document/数据库设计（fan）.xlsx
+++ b/document/数据库设计（fan）.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" activeTab="1"/>
+    <workbookView windowWidth="19095" windowHeight="8865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="商户信息表" sheetId="1" r:id="rId1"/>
     <sheet name="管理员任务表" sheetId="2" r:id="rId2"/>
-    <sheet name="管理员信息表" sheetId="3" r:id="rId3"/>
-    <sheet name="用户信息表" sheetId="4" r:id="rId4"/>
+    <sheet name="用户信息表" sheetId="3" r:id="rId3"/>
+    <sheet name="管理员信息表" sheetId="4" r:id="rId4"/>
     <sheet name="收藏信息表" sheetId="5" r:id="rId5"/>
     <sheet name="评论信息表" sheetId="6" r:id="rId6"/>
     <sheet name="教师信息表" sheetId="7" r:id="rId7"/>
@@ -450,6 +450,84 @@
     <t>创建管理员名字</t>
   </si>
   <si>
+    <t>表名</t>
+  </si>
+  <si>
+    <t>用户信息表</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>user_login_times</t>
+  </si>
+  <si>
+    <t>user_nickname</t>
+  </si>
+  <si>
+    <t>user_realname</t>
+  </si>
+  <si>
+    <t>user_email</t>
+  </si>
+  <si>
+    <t>user_password</t>
+  </si>
+  <si>
+    <t>user_mobile</t>
+  </si>
+  <si>
+    <t>user_current_school</t>
+  </si>
+  <si>
+    <t>user_current_major</t>
+  </si>
+  <si>
+    <t>user_target_school</t>
+  </si>
+  <si>
+    <t>user_target_major</t>
+  </si>
+  <si>
+    <t>user_target_area</t>
+  </si>
+  <si>
+    <t>user_language_level</t>
+  </si>
+  <si>
+    <t>user_identitynumber</t>
+  </si>
+  <si>
+    <t>user_config</t>
+  </si>
+  <si>
+    <t>user_follower</t>
+  </si>
+  <si>
+    <t>user_read_history</t>
+  </si>
+  <si>
+    <t>user_favourate</t>
+  </si>
+  <si>
+    <t>user_purchased</t>
+  </si>
+  <si>
+    <t>user_group</t>
+  </si>
+  <si>
+    <t>user_email_confirm</t>
+  </si>
+  <si>
+    <t>user_id_verification</t>
+  </si>
+  <si>
+    <t>user_special_identification</t>
+  </si>
+  <si>
+    <t>user_create_time</t>
+  </si>
+  <si>
     <t>管理员姓名</t>
   </si>
   <si>
@@ -481,84 +559,6 @@
   </si>
   <si>
     <t>是否已经删除</t>
-  </si>
-  <si>
-    <t>表名</t>
-  </si>
-  <si>
-    <t>用户信息表</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>user_login_times</t>
-  </si>
-  <si>
-    <t>user_nickname</t>
-  </si>
-  <si>
-    <t>user_realname</t>
-  </si>
-  <si>
-    <t>user_email</t>
-  </si>
-  <si>
-    <t>user_password</t>
-  </si>
-  <si>
-    <t>user_mobile</t>
-  </si>
-  <si>
-    <t>user_current_school</t>
-  </si>
-  <si>
-    <t>user_current_major</t>
-  </si>
-  <si>
-    <t>user_target_school</t>
-  </si>
-  <si>
-    <t>user_target_major</t>
-  </si>
-  <si>
-    <t>user_target_area</t>
-  </si>
-  <si>
-    <t>user_language_level</t>
-  </si>
-  <si>
-    <t>user_identitynumber</t>
-  </si>
-  <si>
-    <t>user_config</t>
-  </si>
-  <si>
-    <t>user_follower</t>
-  </si>
-  <si>
-    <t>user_read_history</t>
-  </si>
-  <si>
-    <t>user_favourate</t>
-  </si>
-  <si>
-    <t>user_purchased</t>
-  </si>
-  <si>
-    <t>user_group</t>
-  </si>
-  <si>
-    <t>user_email_confirm</t>
-  </si>
-  <si>
-    <t>user_id_verification</t>
-  </si>
-  <si>
-    <t>user_special_identification</t>
-  </si>
-  <si>
-    <t>user_create_time</t>
   </si>
 </sst>
 </file>
@@ -567,9 +567,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -588,6 +588,88 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -603,61 +685,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -687,17 +717,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -710,27 +731,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -741,43 +741,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,139 +921,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,34 +937,19 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -981,6 +966,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,8 +1003,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1027,8 +1027,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1040,10 +1040,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1052,133 +1052,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2158,7 +2158,7 @@
   <sheetPr/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2364,6 +2364,282 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="40.375" customWidth="1"/>
+    <col min="6" max="6" width="61.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:F10"/>
@@ -2406,10 +2682,10 @@
         <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2420,10 +2696,10 @@
         <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2434,7 +2710,7 @@
         <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2445,18 +2721,18 @@
         <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2477,304 +2753,28 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
         <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:F27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="40.375" customWidth="1"/>
-    <col min="6" max="6" width="61.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
 </file>

</xml_diff>